<commit_message>
fixing date typo in 0648
</commit_message>
<xml_diff>
--- a/library/library_0648.xlsx
+++ b/library/library_0648.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">GCAACGC</t>
   </si>
   <si>
-    <t xml:space="preserve">12.010.11</t>
+    <t xml:space="preserve">12.10.11</t>
   </si>
   <si>
     <t xml:space="preserve">TGATTAC</t>
@@ -233,16 +233,16 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="9" style="0" width="8.67"/>

</xml_diff>